<commit_message>
Added Method and xpath for History and Transaction at spark cloud
</commit_message>
<xml_diff>
--- a/HuskPowerSystem/resource/sparkmeterdata.xlsx
+++ b/HuskPowerSystem/resource/sparkmeterdata.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\Pradeep\CoreJavaPractice\HuskPowerSystem\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monocept\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5144B5-27E1-4C7D-826A-B954A2084599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6967E0-2052-4D0C-9C3E-7CBE958CF083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DF3DC22E-1FFC-4195-B0B5-A2E2016C89D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DF3DC22E-1FFC-4195-B0B5-A2E2016C89D5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="SparkData" sheetId="2" r:id="rId2"/>
+    <sheet name="SparkData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="87">
   <si>
     <t>PlantCode</t>
   </si>
@@ -660,625 +659,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E1B996-1FBA-4A3A-9C9B-2F2BA13446F2}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67259727-0673-4BB8-A6A0-D4CCDAC0D9BC}">
-  <dimension ref="A1:D42"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1289,10 +679,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1303,10 +693,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1317,10 +707,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1331,10 +721,10 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1345,10 +735,10 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1359,10 +749,10 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1373,10 +763,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,10 +777,10 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,10 +791,10 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1415,10 +805,10 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1429,10 +819,10 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1443,10 +833,10 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1457,10 +847,10 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1471,10 +861,10 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1485,10 +875,10 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1499,10 +889,10 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1513,10 +903,10 @@
         <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1527,10 +917,10 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1541,10 +931,10 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,10 +945,10 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1569,10 +959,10 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1583,10 +973,10 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1597,10 +987,10 @@
         <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,10 +1001,10 @@
         <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1625,10 +1015,10 @@
         <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1639,10 +1029,10 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1653,10 +1043,10 @@
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1667,10 +1057,10 @@
         <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,10 +1071,10 @@
         <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,10 +1085,10 @@
         <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1709,10 +1099,10 @@
         <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,10 +1113,10 @@
         <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,10 +1127,10 @@
         <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1751,10 +1141,10 @@
         <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1765,10 +1155,10 @@
         <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1779,10 +1169,10 @@
         <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1793,10 +1183,10 @@
         <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1807,10 +1197,10 @@
         <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1821,10 +1211,10 @@
         <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,10 +1225,10 @@
         <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1849,10 +1239,10 @@
         <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,10 +1253,10 @@
         <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>